<commit_message>
Maga (Sin la Skin)
</commit_message>
<xml_diff>
--- a/Rogue-Lite/Assets/Game/Resources/NPCs/Camp2.xlsx
+++ b/Rogue-Lite/Assets/Game/Resources/NPCs/Camp2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="304">
   <si>
     <t>Index</t>
   </si>
@@ -38,36 +38,87 @@
     <t>Maga apasionada</t>
   </si>
   <si>
-    <t>Buenas, caballero, soy la maga.</t>
+    <t>Greetins, knight, I'm a magician.</t>
+  </si>
+  <si>
+    <t>Buenas, caballero, soy una maga del norte.</t>
+  </si>
+  <si>
+    <t>Sei gegrüßt, Ritter. Ich bin die Zauberin.</t>
+  </si>
+  <si>
+    <t>I've heard about your attempts of trying to reach the end of the cave.</t>
   </si>
   <si>
     <t>He escuchado acerca de vuestros intentos de llegar al final de la cueva.</t>
   </si>
   <si>
+    <t>Ich habe gehört du hast versucht das Ende der Höhle zu erreichen.</t>
+  </si>
+  <si>
+    <t>As you might have guessed already, there is something in this place that escapes the understanding of man itself.</t>
+  </si>
+  <si>
     <t>Te lo habrás podido imaginar, pero hay algo en ese lugar que escapa al entendimiento de todo hombre.</t>
   </si>
   <si>
+    <t>Wie Sie vielleicht schon erraten haben, gibt es an diesem Ort etwas das dem Verstädnis des Menschen selbst entegeht.</t>
+  </si>
+  <si>
+    <t>Or at least it does for those who lack magical knowledge.</t>
+  </si>
+  <si>
     <t>Al menos, a cualquiera que no posea conocimientos sobre magia.</t>
   </si>
   <si>
+    <t>Oder zumindest für diejenigen, denen das magische Wissen fehlt.</t>
+  </si>
+  <si>
+    <t>You know what? We could make a deal.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Podemos llegar a un trato. </t>
   </si>
   <si>
+    <t>Wir können eine Vereinbarung treffen.</t>
+  </si>
+  <si>
+    <t>If you have got the coin for it, I'll strenghten your abilities. In other words: You'll be stronger.</t>
+  </si>
+  <si>
     <t>Si me pagas, fortaleceré tus cualidades, haciéndote más poderoso.</t>
   </si>
   <si>
+    <t>Wenn Sie das Gold haben, werde ich Ihre Fähigkeiten stärken. Mit anderen Worten, Sie werden stärker sein.</t>
+  </si>
+  <si>
+    <t>This should make your life in the cave a little bit easier.</t>
+  </si>
+  <si>
     <t>Así podrás llegar más lejos en tu aventura.</t>
   </si>
   <si>
+    <t>Das wird Ihre Leben in der Höhle ein bisschen einfacher machen.</t>
+  </si>
+  <si>
+    <t>Come on, take a look.</t>
+  </si>
+  <si>
     <t>Vamos, acércate.</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Komm schon, schau mal.</t>
+  </si>
+  <si>
+    <t>Good luck, knight.</t>
   </si>
   <si>
     <t>Buena suerte, caballero.</t>
   </si>
   <si>
+    <t>Viel Glück, Ritter.</t>
+  </si>
+  <si>
     <t>Magic is a fascinating discipline.</t>
   </si>
   <si>
@@ -95,9 +146,15 @@
     <t>Schauen Sie mal rein und sagen Sie mir, ob Sie etwas interessiert</t>
   </si>
   <si>
+    <t>Have a nice crusade.</t>
+  </si>
+  <si>
     <t>Buena cruzada.</t>
   </si>
   <si>
+    <t>Ich wünsche Ihnen einen schönen Kreuzzug.</t>
+  </si>
+  <si>
     <t>La magia de la cueva</t>
   </si>
   <si>
@@ -137,9 +194,15 @@
     <t>Hahaha, vergib mir meine Begeisterung. Was brauchst du?</t>
   </si>
   <si>
+    <t>Good luck.</t>
+  </si>
+  <si>
     <t>Buena suerte.</t>
   </si>
   <si>
+    <t>Viel Glück.</t>
+  </si>
+  <si>
     <t>Interés por la cueva</t>
   </si>
   <si>
@@ -188,9 +251,15 @@
     <t>Was willst du?</t>
   </si>
   <si>
+    <t>Be back soon.</t>
+  </si>
+  <si>
     <t>No tardes en volver.</t>
   </si>
   <si>
+    <t>Kommen Sie bald wieder zurück.</t>
+  </si>
+  <si>
     <t>Aplicar la magia de la cueva a sus objetos</t>
   </si>
   <si>
@@ -230,9 +299,15 @@
     <t>Brauchst du etwas?</t>
   </si>
   <si>
+    <t>May the power of the source protect you.</t>
+  </si>
+  <si>
     <t>Que la magia de la fuente te protega.</t>
   </si>
   <si>
+    <t>Möge die Magie der Quelle Sie beschützen</t>
+  </si>
+  <si>
     <t>Le agradece por sus anteriores compras</t>
   </si>
   <si>
@@ -242,18 +317,36 @@
     <t>Me alegro de que confíes en mis hechizos, te serán de gran utilidad.</t>
   </si>
   <si>
+    <t>Ich bin froh, dass Sie meinen Zabersprüchen vetrauen, sie werden von großen nutzen sein.</t>
+  </si>
+  <si>
     <t>If you have any questions, ask me.</t>
   </si>
   <si>
     <t>Si tienes cualquier duda, pregúntame.</t>
   </si>
   <si>
-    <t>Dime, qué necesitas.</t>
+    <t>Wenn Sie Fragen haben, fragen Sie mich bitte.</t>
+  </si>
+  <si>
+    <t>Tell me, what do you need?</t>
+  </si>
+  <si>
+    <t>Dime, ¿qué necesitas?</t>
+  </si>
+  <si>
+    <t>Was brauchen Sie?</t>
+  </si>
+  <si>
+    <t>I'll be waiting for your arrival.</t>
   </si>
   <si>
     <t>Estaré esperando tu regreso.</t>
   </si>
   <si>
+    <t>Ich werde auf Ihre Ankunft warten.</t>
+  </si>
+  <si>
     <t>Presentación del personaje, con voz pícara.</t>
   </si>
   <si>
@@ -434,22 +527,34 @@
     <t>Elige las prendas que más te gusten.</t>
   </si>
   <si>
+    <t>Wähle einen deiner Vorlieben, Liebling.</t>
+  </si>
+  <si>
     <t>Alrighty, who am I to judge? Be back as soon as you can!  &lt;bounce&gt;^3^</t>
   </si>
   <si>
     <t>Mmmm, bueno, si te gusta ir así, adelante. ¡No tardes en volver!  &lt;bounce&gt;^3^</t>
   </si>
   <si>
+    <t>Mmm, in Ordnung, wenn es dir gefällt, wer bin ich zu beurteilen? Komm zurück so bald wie möglich!</t>
+  </si>
+  <si>
     <t>Hey, you still alive! &lt;bounce&gt;°ロ°</t>
   </si>
   <si>
     <t>¡Ay, sigues vivo! &lt;bounce&gt;°ロ°</t>
   </si>
   <si>
+    <t>Oh, du bist noch am Leben!</t>
+  </si>
+  <si>
     <t>It is my pleasure to see you again, honey.</t>
   </si>
   <si>
-    <t>Qué ilusión volver a verte {shake}(ง ͠° ͟ل͜ ͡°)ง</t>
+    <t>Qué ilusión volver a verte.</t>
+  </si>
+  <si>
+    <t>Es ist mir eine Freue dich wiederzusehen.</t>
   </si>
   <si>
     <t>Come come don't be shy, take a look. It's all four you. &lt;bounce&gt;( ͡° ͜ʖ ͡°)</t>
@@ -458,7 +563,10 @@
     <t>Venga, mira todo lo que tengo. Es todo para tí. &lt;bounce&gt;( ͡° ͜ʖ ͡°)</t>
   </si>
   <si>
-    <t>Hace a nice crusade! &lt;bounce&gt;ʢoᴥoʡ</t>
+    <t>Komm schon, schau was ich auf Lager habe. Es ist alles für dich.</t>
+  </si>
+  <si>
+    <t>Have a nice crusade! &lt;bounce&gt;ʢoᴥoʡ</t>
   </si>
   <si>
     <t>Que pases una buena cruzada. &lt;bounce&gt;ʢoᴥoʡ</t>
@@ -479,96 +587,171 @@
     <t>Soy el armero. El mismo... en armadura y hueso.</t>
   </si>
   <si>
+    <t>By the gods, kid. Going into that cave has left you whacked.</t>
+  </si>
+  <si>
     <t>¡Diablos pequeñín! Entrar en esa cueva te ha sentado mal.</t>
   </si>
   <si>
     <t>Los aventureros que entran en ella aseguran haber muerto.</t>
   </si>
   <si>
+    <t>All I see are cowards, cowards that only try to escape at glance of a challenge.</t>
+  </si>
+  <si>
     <t>Pero lo que yo veo es a una panda de cobardes sin agallas que se dedican a huir.</t>
   </si>
   <si>
+    <t>Mmm... Something is troubling you, I can see it in your eyes.</t>
+  </si>
+  <si>
     <t>Mmm... noto la confusión en tu mirada.</t>
   </si>
   <si>
+    <t>Look, kid. If you bring me the coin I can forge you brand new weapons. Come closer, take a look at this piece here.</t>
+  </si>
+  <si>
     <t>Mira, si obtienes oro me puedes pagar para que te forje nuevas armas. Te las enseño.</t>
   </si>
   <si>
+    <t>Good luck, kid.</t>
+  </si>
+  <si>
     <t>Buena suerte, canijo.</t>
   </si>
   <si>
     <t>Segundo encuentro</t>
   </si>
   <si>
+    <t>Welcome back, kid.</t>
+  </si>
+  <si>
     <t>Bienvenido de nuevo.</t>
   </si>
   <si>
+    <t>Well well, kid. I can see you have gotten some use out of that weapon I gave you.</t>
+  </si>
+  <si>
     <t>Veo que sabes aprovechar bien tu arma.</t>
   </si>
   <si>
+    <t>What if I told you I could make it even deadlier?</t>
+  </si>
+  <si>
     <t>¿Y si te dijera que te puedo ofrecer algo mucho mejor...?</t>
   </si>
   <si>
+    <t>Enjoy it but be careful, you seem rather quiet but I bet you are as sharp as your iron.</t>
+  </si>
+  <si>
     <t>Disfrútala y ten cuidado con lo que hagas con ella, te veo callado, pero peligroso.</t>
   </si>
   <si>
+    <t>Have a nice crusade, kid.</t>
+  </si>
+  <si>
     <t>Buena cruzada enano.</t>
   </si>
   <si>
     <t>Tercer encuentro</t>
   </si>
   <si>
+    <t>By the gods, look at you! You are one hell of a soldier.</t>
+  </si>
+  <si>
     <t>Oh, mírate, estás hecho todo un guerrero.</t>
   </si>
   <si>
+    <t>Come here, even the finest of weapons needs a whetstone from time to time.</t>
+  </si>
+  <si>
     <t>Aunque todo buen guerrero necesita mejorar sus armas.</t>
   </si>
   <si>
+    <t>Allow me to take a look at our girl.</t>
+  </si>
+  <si>
     <t>Ven, ven, no te cortes.</t>
   </si>
   <si>
+    <t>Go give 'em hell, kid.</t>
+  </si>
+  <si>
     <t>Carga contra tus enemigos sin miedo.</t>
   </si>
   <si>
     <t>Cuarto encuentro</t>
   </si>
   <si>
+    <t>Oh, you are back.</t>
+  </si>
+  <si>
     <t>Vaya, has vuelto.</t>
   </si>
   <si>
+    <t>And you are... all covered in mud and blood.</t>
+  </si>
+  <si>
     <t>Y veo que estás cubierto de tuétano.</t>
   </si>
   <si>
+    <t>I'm glad you are putting them to good use.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jajaja... Sacándole partido a mis armas por lo que veo. </t>
   </si>
   <si>
+    <t>So, what is it gonna be this time, kid?</t>
+  </si>
+  <si>
     <t>Así me gusta. Vamos, no te cortes, dime, ¿qué necesitas?</t>
   </si>
   <si>
+    <t>Let's go, kid.</t>
+  </si>
+  <si>
     <t>A tope, canijo.</t>
   </si>
   <si>
     <t>Quinto encuentro</t>
   </si>
   <si>
+    <t>You never stop surprising me, kid.</t>
+  </si>
+  <si>
     <t>Cada vez me sorprendes más chaval.</t>
   </si>
   <si>
+    <t>You either are too good at this or do have a deathwish.</t>
+  </si>
+  <si>
     <t>O esto se te da demasiado bien o eres muy estúpido.</t>
   </si>
   <si>
+    <t>Not many people come out of that cave alive and want to get back in again.</t>
+  </si>
+  <si>
     <t>A poca gente he visto entrar más de dos veces en esa cueva y querer volver.</t>
   </si>
   <si>
+    <t>Anyway, kid. If you are planning on returning to that hole, you better arm yourself to the teeth.</t>
+  </si>
+  <si>
     <t>En fin canijo, si vas a volver ármate bien.</t>
   </si>
   <si>
+    <t>Good luck my mute friend.</t>
+  </si>
+  <si>
     <t>Suerte mi mudo amigo.</t>
   </si>
   <si>
     <t>Sexto encuentro</t>
   </si>
   <si>
+    <t>Oh, welcome back.</t>
+  </si>
+  <si>
     <t>Oh, bienenido de nuevo.</t>
   </si>
   <si>
@@ -584,7 +767,7 @@
     <t>Te estaré esperando para cuando necesites una arma nueva.</t>
   </si>
   <si>
-    <t>¡Alabado sean los dioses!</t>
+    <t>¡Alabados sean los dioses!</t>
   </si>
   <si>
     <t>¡Adiós!</t>
@@ -763,10 +946,11 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -783,6 +967,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC27BA0"/>
+        <bgColor rgb="FFC27BA0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5A6BD"/>
+        <bgColor rgb="FFD5A6BD"/>
       </patternFill>
     </fill>
     <fill>
@@ -804,7 +1000,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -815,6 +1011,12 @@
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -832,7 +1034,7 @@
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -844,19 +1046,19 @@
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1098,7 +1300,7 @@
     <col customWidth="1" min="3" max="3" width="47.43"/>
     <col customWidth="1" min="4" max="4" width="99.86"/>
     <col customWidth="1" min="5" max="5" width="95.14"/>
-    <col customWidth="1" min="6" max="6" width="102.71"/>
+    <col customWidth="1" min="6" max="6" width="105.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1131,11 +1333,15 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -1145,11 +1351,15 @@
         <v>1.0</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
@@ -1159,11 +1369,15 @@
         <v>1.0</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
@@ -1173,11 +1387,15 @@
         <v>1.0</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
@@ -1187,11 +1405,15 @@
         <v>1.0</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
@@ -1201,455 +1423,493 @@
         <v>1.0</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>7.0</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <v>1.0</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="4">
+      <c r="A9" s="6">
         <v>8.0</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="7">
         <v>1.0</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="6"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="4">
+      <c r="A10" s="6">
         <v>9.0</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="7">
         <v>1.0</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="7"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="4">
+      <c r="A11" s="6">
         <v>10.0</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="10">
         <v>2.0</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>19</v>
+      <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4">
+      <c r="A12" s="6">
         <v>11.0</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="10">
         <v>2.0</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>22</v>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4">
+      <c r="A13" s="6">
         <v>12.0</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="7">
         <v>2.0</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>25</v>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4">
+      <c r="A14" s="6">
         <v>13.0</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="10">
         <v>2.0</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="6"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="4">
+      <c r="A15" s="6">
         <v>14.0</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="10">
         <v>3.0</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>30</v>
+      <c r="C15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4">
+      <c r="A16" s="6">
         <v>15.0</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="10">
         <v>3.0</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>33</v>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4">
+      <c r="A17" s="6">
         <v>16.0</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="10">
         <v>3.0</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>36</v>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4">
+      <c r="A18" s="6">
         <v>17.0</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="7">
         <v>3.0</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>39</v>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4">
+      <c r="A19" s="6">
         <v>18.0</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="10">
         <v>3.0</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="6"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="4">
+      <c r="A20" s="6">
         <v>19.0</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="10">
         <v>4.0</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>44</v>
+      <c r="C20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4">
+      <c r="A21" s="6">
         <v>20.0</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="10">
         <v>4.0</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>47</v>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4">
+      <c r="A22" s="6">
         <v>21.0</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="10">
         <v>4.0</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>50</v>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4">
+      <c r="A23" s="6">
         <v>22.0</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="10">
         <v>4.0</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>53</v>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4">
+      <c r="A24" s="6">
         <v>23.0</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="7">
         <v>4.0</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>56</v>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4">
+      <c r="A25" s="6">
         <v>24.0</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="10">
         <v>4.0</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="6"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="4">
+      <c r="A26" s="6">
         <v>25.0</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="10">
         <v>5.0</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>61</v>
+      <c r="C26" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4">
+      <c r="A27" s="6">
         <v>26.0</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="10">
         <v>5.0</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>64</v>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4">
+      <c r="A28" s="6">
         <v>27.0</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="10">
         <v>5.0</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>67</v>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4">
+      <c r="A29" s="6">
         <v>28.0</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="7">
         <v>5.0</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>70</v>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4">
+      <c r="A30" s="6">
         <v>29.0</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="7">
         <v>5.0</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="6"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="4">
+      <c r="A31" s="6">
         <v>30.0</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="10">
         <v>6.0</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="6"/>
+      <c r="C31" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="4">
+      <c r="A32" s="6">
         <v>31.0</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="10">
         <v>6.0</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F32" s="6"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
         <v>32.0</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="10">
         <v>6.0</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" s="6"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
@@ -1659,11 +1919,15 @@
         <v>6.0</v>
       </c>
       <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E34" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F34" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2"/>
@@ -1758,7 +2022,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1770,15 +2034,15 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="11"/>
+        <v>112</v>
+      </c>
+      <c r="F2" s="13"/>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -1789,12 +2053,12 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="11"/>
+        <v>114</v>
+      </c>
+      <c r="F3" s="13"/>
     </row>
     <row r="4">
       <c r="A4" s="2">
@@ -1805,12 +2069,12 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="11"/>
+        <v>116</v>
+      </c>
+      <c r="F4" s="13"/>
     </row>
     <row r="5">
       <c r="A5" s="2">
@@ -1821,12 +2085,12 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" s="11"/>
+        <v>118</v>
+      </c>
+      <c r="F5" s="13"/>
     </row>
     <row r="6">
       <c r="A6" s="2">
@@ -1837,12 +2101,12 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="11"/>
+        <v>119</v>
+      </c>
+      <c r="F6" s="13"/>
     </row>
     <row r="7">
       <c r="A7" s="2">
@@ -1852,15 +2116,15 @@
         <v>2.0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="11"/>
+        <v>122</v>
+      </c>
+      <c r="F7" s="13"/>
     </row>
     <row r="8">
       <c r="A8" s="2">
@@ -1871,12 +2135,12 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="11"/>
+        <v>124</v>
+      </c>
+      <c r="F8" s="13"/>
     </row>
     <row r="9">
       <c r="A9" s="2">
@@ -1887,12 +2151,12 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="11"/>
+        <v>126</v>
+      </c>
+      <c r="F9" s="13"/>
     </row>
     <row r="10">
       <c r="A10" s="2">
@@ -1902,15 +2166,15 @@
         <v>3.0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="11"/>
+        <v>129</v>
+      </c>
+      <c r="F10" s="13"/>
     </row>
     <row r="11">
       <c r="A11" s="2">
@@ -1921,12 +2185,12 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="11"/>
+        <v>131</v>
+      </c>
+      <c r="F11" s="13"/>
     </row>
     <row r="12">
       <c r="A12" s="2">
@@ -1937,12 +2201,12 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="11"/>
+        <v>133</v>
+      </c>
+      <c r="F12" s="13"/>
     </row>
     <row r="13">
       <c r="A13" s="2">
@@ -1953,12 +2217,12 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="11"/>
+        <v>135</v>
+      </c>
+      <c r="F13" s="13"/>
     </row>
     <row r="14">
       <c r="A14" s="2">
@@ -1969,12 +2233,12 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="11"/>
+        <v>137</v>
+      </c>
+      <c r="F14" s="13"/>
     </row>
     <row r="15">
       <c r="A15" s="2">
@@ -1985,12 +2249,12 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="11"/>
+        <v>139</v>
+      </c>
+      <c r="F15" s="13"/>
     </row>
     <row r="16">
       <c r="A16" s="2">
@@ -2001,12 +2265,12 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="11"/>
+        <v>141</v>
+      </c>
+      <c r="F16" s="13"/>
     </row>
     <row r="17">
       <c r="A17" s="2">
@@ -2016,15 +2280,15 @@
         <v>5.0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F17" s="11"/>
+        <v>144</v>
+      </c>
+      <c r="F17" s="13"/>
     </row>
     <row r="18">
       <c r="A18" s="2">
@@ -2035,12 +2299,12 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="11"/>
+        <v>145</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" s="13"/>
     </row>
     <row r="19">
       <c r="A19" s="2">
@@ -2051,12 +2315,12 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F19" s="11"/>
+        <v>148</v>
+      </c>
+      <c r="F19" s="13"/>
     </row>
     <row r="20">
       <c r="A20" s="2">
@@ -2067,12 +2331,12 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F20" s="11"/>
+        <v>150</v>
+      </c>
+      <c r="F20" s="13"/>
     </row>
     <row r="21">
       <c r="A21" s="2"/>
@@ -2080,7 +2344,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="11"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22">
       <c r="A22" s="2"/>
@@ -2088,7 +2352,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="11"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23">
       <c r="A23" s="2"/>
@@ -2096,7 +2360,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="11"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24">
       <c r="A24" s="2"/>
@@ -2104,7 +2368,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="11"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25">
       <c r="A25" s="2"/>
@@ -2112,7 +2376,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="11"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26">
       <c r="A26" s="2"/>
@@ -2120,7 +2384,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="11"/>
+      <c r="F26" s="13"/>
     </row>
     <row r="27">
       <c r="A27" s="2"/>
@@ -2128,7 +2392,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="11"/>
+      <c r="F27" s="13"/>
     </row>
     <row r="28">
       <c r="A28" s="2"/>
@@ -2136,7 +2400,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="11"/>
+      <c r="F28" s="13"/>
     </row>
     <row r="29">
       <c r="A29" s="2"/>
@@ -2144,7 +2408,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="11"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30">
       <c r="A30" s="2"/>
@@ -2152,7 +2416,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="11"/>
+      <c r="F30" s="13"/>
     </row>
     <row r="31">
       <c r="A31" s="2"/>
@@ -2160,7 +2424,7 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="11"/>
+      <c r="F31" s="13"/>
     </row>
     <row r="32">
       <c r="A32" s="2"/>
@@ -2168,7 +2432,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="11"/>
+      <c r="F32" s="13"/>
     </row>
     <row r="33">
       <c r="A33" s="2"/>
@@ -2176,7 +2440,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="11"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34">
       <c r="A34" s="2"/>
@@ -2184,7 +2448,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="11"/>
+      <c r="F34" s="13"/>
     </row>
     <row r="35">
       <c r="A35" s="2"/>
@@ -2192,7 +2456,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="11"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36">
       <c r="A36" s="2"/>
@@ -2200,7 +2464,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="11"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37">
       <c r="A37" s="2"/>
@@ -2208,7 +2472,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="11"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38">
       <c r="A38" s="2"/>
@@ -2216,7 +2480,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="11"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39">
       <c r="A39" s="2"/>
@@ -2224,7 +2488,7 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="11"/>
+      <c r="F39" s="13"/>
     </row>
     <row r="40">
       <c r="A40" s="2"/>
@@ -2232,7 +2496,7 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="11"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41">
       <c r="A41" s="2"/>
@@ -2240,7 +2504,7 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="11"/>
+      <c r="F41" s="13"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2276,7 +2540,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -2289,135 +2553,139 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13">
+      <c r="A2" s="15">
         <v>1.0</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="16">
         <v>1.0</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>124</v>
+      <c r="C2" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13">
+      <c r="A3" s="15">
         <v>2.0</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="16">
         <v>1.0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>127</v>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13">
+      <c r="A4" s="15">
         <v>3.0</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="16">
         <v>1.0</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>130</v>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13">
+      <c r="A5" s="15">
         <v>4.0</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="16">
         <v>1.0</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>133</v>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13">
+      <c r="A6" s="15">
         <v>5.0</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="16">
         <v>1.0</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>136</v>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13">
+      <c r="A7" s="15">
         <v>6.0</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="16">
         <v>1.0</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G7" s="14"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="13">
+      <c r="A8" s="15">
         <v>7.0</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="16">
         <v>1.0</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" s="14"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
@@ -2429,12 +2697,14 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
@@ -2446,12 +2716,14 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
@@ -2463,12 +2735,14 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>181</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
@@ -2480,90 +2754,92 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G12" s="3"/>
+        <v>184</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="14">
+      <c r="A13" s="16">
         <v>12.0</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="16">
         <v>3.0</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14">
-      <c r="A14" s="14">
+      <c r="A14" s="16">
         <v>13.0</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="16">
         <v>3.0</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="15">
-      <c r="A15" s="14">
+      <c r="A15" s="16">
         <v>14.0</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="16">
         <v>3.0</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16">
-      <c r="A16" s="14">
+      <c r="A16" s="16">
         <v>15.0</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="16">
         <v>3.0</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17">
-      <c r="A17" s="14">
+      <c r="A17" s="16">
         <v>16.0</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="16">
         <v>3.0</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18">
-      <c r="A18" s="14">
+      <c r="A18" s="16">
         <v>17.0</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="16">
         <v>3.0</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19">
       <c r="A19" s="2"/>
@@ -2571,8 +2847,8 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20">
       <c r="A20" s="2"/>
@@ -2580,8 +2856,8 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21">
       <c r="A21" s="2"/>
@@ -2589,8 +2865,8 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22">
       <c r="A22" s="2"/>
@@ -2598,8 +2874,8 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23">
       <c r="A23" s="2"/>
@@ -2607,8 +2883,8 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24">
       <c r="A24" s="2"/>
@@ -2616,8 +2892,8 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25">
       <c r="A25" s="2"/>
@@ -2625,8 +2901,8 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26">
       <c r="A26" s="2"/>
@@ -2634,8 +2910,8 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27">
       <c r="A27" s="2"/>
@@ -2643,8 +2919,8 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28">
       <c r="A28" s="2"/>
@@ -2652,8 +2928,8 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29">
       <c r="A29" s="2"/>
@@ -2661,8 +2937,8 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30">
       <c r="A30" s="2"/>
@@ -2670,8 +2946,8 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31">
       <c r="A31" s="2"/>
@@ -2679,8 +2955,8 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32">
       <c r="A32" s="2"/>
@@ -2688,8 +2964,8 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33">
       <c r="A33" s="2"/>
@@ -2697,8 +2973,8 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34">
       <c r="A34" s="2"/>
@@ -2706,8 +2982,8 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35">
       <c r="A35" s="2"/>
@@ -2715,8 +2991,8 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36">
       <c r="A36" s="2"/>
@@ -2724,8 +3000,8 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37">
       <c r="A37" s="2"/>
@@ -2733,8 +3009,8 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38">
       <c r="A38" s="2"/>
@@ -2742,8 +3018,8 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
     </row>
     <row r="39">
       <c r="A39" s="2"/>
@@ -2751,8 +3027,8 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40">
       <c r="A40" s="2"/>
@@ -2760,8 +3036,8 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
     </row>
     <row r="41">
       <c r="A41" s="2"/>
@@ -2769,8 +3045,8 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2789,7 +3065,7 @@
   <cols>
     <col customWidth="1" min="3" max="3" width="43.43"/>
     <col customWidth="1" min="4" max="4" width="18.29"/>
-    <col customWidth="1" min="5" max="5" width="88.29"/>
+    <col customWidth="1" min="5" max="5" width="102.29"/>
     <col customWidth="1" min="6" max="6" width="110.57"/>
     <col customWidth="1" min="7" max="7" width="110.71"/>
   </cols>
@@ -2805,7 +3081,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -2818,130 +3094,140 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13">
+      <c r="A2" s="15">
         <v>1.0</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="16">
         <v>1.0</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="14"/>
+      <c r="C2" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="16"/>
     </row>
     <row r="3">
-      <c r="A3" s="13">
+      <c r="A3" s="15">
         <v>2.0</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="16">
         <v>1.0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="G3" s="14"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="13">
+      <c r="A4" s="15">
         <v>3.0</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="16">
         <v>1.0</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="G4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" s="17"/>
     </row>
     <row r="5">
-      <c r="A5" s="13">
+      <c r="A5" s="15">
         <v>4.0</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="16">
         <v>1.0</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="G5" s="14"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="G5" s="16"/>
     </row>
     <row r="6">
-      <c r="A6" s="13">
+      <c r="A6" s="15">
         <v>5.0</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="16">
         <v>1.0</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="G6" s="14"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" s="16"/>
     </row>
     <row r="7">
-      <c r="A7" s="13">
+      <c r="A7" s="15">
         <v>6.0</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="16">
         <v>1.0</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7" s="14"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" s="16"/>
     </row>
     <row r="8">
-      <c r="A8" s="13">
+      <c r="A8" s="15">
         <v>7.0</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="16">
         <v>1.0</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="G8" s="14"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G8" s="16"/>
     </row>
     <row r="9">
-      <c r="A9" s="13">
+      <c r="A9" s="15">
         <v>8.0</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="16">
         <v>1.0</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G9" s="14"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="G9" s="16"/>
     </row>
     <row r="10">
       <c r="A10" s="2">
@@ -2951,12 +3237,14 @@
         <v>2.0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>160</v>
+        <v>201</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>202</v>
+      </c>
       <c r="F10" s="3" t="s">
-        <v>161</v>
+        <v>203</v>
       </c>
       <c r="G10" s="3"/>
     </row>
@@ -2969,9 +3257,11 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="F11" s="3" t="s">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="G11" s="3"/>
     </row>
@@ -2984,9 +3274,11 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="F12" s="3" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="G12" s="3"/>
     </row>
@@ -2999,9 +3291,11 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="F13" s="3" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -3014,73 +3308,83 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="F14" s="3" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="13">
+      <c r="A15" s="15">
         <v>14.0</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="16">
         <v>3.0</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="G15" s="17"/>
+      <c r="C15" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="G15" s="19"/>
     </row>
     <row r="16">
-      <c r="A16" s="13">
+      <c r="A16" s="15">
         <v>15.0</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="16">
         <v>3.0</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="G16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="G16" s="19"/>
     </row>
     <row r="17">
-      <c r="A17" s="13">
+      <c r="A17" s="15">
         <v>16.0</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="16">
         <v>3.0</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="G17" s="17"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="G17" s="19"/>
     </row>
     <row r="18">
-      <c r="A18" s="13">
+      <c r="A18" s="15">
         <v>17.0</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="16">
         <v>3.0</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="G18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="G18" s="19"/>
     </row>
     <row r="19">
       <c r="A19" s="2">
@@ -3090,14 +3394,16 @@
         <v>4.0</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="G19" s="6"/>
+      <c r="E19" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G19" s="8"/>
     </row>
     <row r="20">
       <c r="A20" s="2">
@@ -3108,11 +3414,13 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="G20" s="6"/>
+      <c r="E20" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="G20" s="8"/>
     </row>
     <row r="21">
       <c r="A21" s="2">
@@ -3123,11 +3431,13 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G21" s="6"/>
+      <c r="E21" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="G21" s="8"/>
     </row>
     <row r="22">
       <c r="A22" s="2">
@@ -3138,11 +3448,13 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G22" s="7"/>
+      <c r="E22" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="G22" s="9"/>
     </row>
     <row r="23">
       <c r="A23" s="2">
@@ -3153,88 +3465,100 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="G23" s="7"/>
+      <c r="E23" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G23" s="9"/>
     </row>
     <row r="24">
-      <c r="A24" s="13">
+      <c r="A24" s="15">
         <v>23.0</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="16">
         <v>5.0</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="G24" s="14"/>
+      <c r="C24" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="G24" s="16"/>
     </row>
     <row r="25">
-      <c r="A25" s="13">
+      <c r="A25" s="15">
         <v>24.0</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="16">
         <v>5.0</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="G25" s="14"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="G25" s="16"/>
     </row>
     <row r="26">
-      <c r="A26" s="13">
+      <c r="A26" s="15">
         <v>25.0</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="16">
         <v>5.0</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="G26" s="14"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="G26" s="16"/>
     </row>
     <row r="27">
-      <c r="A27" s="13">
+      <c r="A27" s="15">
         <v>26.0</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="16">
         <v>5.0</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="G27" s="14"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="G27" s="16"/>
     </row>
     <row r="28">
-      <c r="A28" s="13">
+      <c r="A28" s="15">
         <v>27.0</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="16">
         <v>5.0</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="G28" s="14"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="G28" s="16"/>
     </row>
     <row r="29">
       <c r="A29" s="2">
@@ -3244,12 +3568,14 @@
         <v>6.0</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>183</v>
+        <v>243</v>
       </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>244</v>
+      </c>
       <c r="F29" s="3" t="s">
-        <v>184</v>
+        <v>245</v>
       </c>
       <c r="G29" s="3"/>
     </row>
@@ -3264,7 +3590,7 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>185</v>
+        <v>246</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -3279,7 +3605,7 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>186</v>
+        <v>247</v>
       </c>
       <c r="G31" s="3"/>
     </row>
@@ -3294,7 +3620,7 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>187</v>
+        <v>248</v>
       </c>
       <c r="G32" s="3"/>
     </row>
@@ -3309,39 +3635,39 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>188</v>
+        <v>249</v>
       </c>
       <c r="G33" s="3"/>
     </row>
     <row r="34">
-      <c r="A34" s="13">
+      <c r="A34" s="15">
         <v>33.0</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="16">
         <v>7.0</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="G34" s="14"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="G34" s="16"/>
     </row>
     <row r="35">
-      <c r="A35" s="13">
+      <c r="A35" s="15">
         <v>34.0</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="16">
         <v>7.0</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="G35" s="14"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="G35" s="16"/>
     </row>
     <row r="36">
       <c r="A36" s="2"/>
@@ -3430,7 +3756,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -3443,141 +3769,141 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13">
+      <c r="A2" s="15">
         <v>1.0</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="16">
         <v>1.0</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="G2" s="14"/>
+      <c r="C2" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="G2" s="16"/>
     </row>
     <row r="3">
-      <c r="A3" s="13">
+      <c r="A3" s="15">
         <v>2.0</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="16">
         <v>1.0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="G3" s="14"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="13">
+      <c r="A4" s="15">
         <v>3.0</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="16">
         <v>1.0</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="G4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="G4" s="17"/>
     </row>
     <row r="5">
-      <c r="A5" s="13">
+      <c r="A5" s="15">
         <v>4.0</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="16">
         <v>1.0</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="G5" s="14"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="G5" s="16"/>
     </row>
     <row r="6">
-      <c r="A6" s="13">
+      <c r="A6" s="15">
         <v>5.0</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="16">
         <v>1.0</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="G6" s="14"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="G6" s="16"/>
     </row>
     <row r="7">
-      <c r="A7" s="13">
+      <c r="A7" s="15">
         <v>6.0</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="16">
         <v>1.0</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="G7" s="14"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="G7" s="16"/>
     </row>
     <row r="8">
-      <c r="A8" s="13">
+      <c r="A8" s="15">
         <v>7.0</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="16">
         <v>1.0</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="G8" s="14"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="G8" s="16"/>
     </row>
     <row r="9">
-      <c r="A9" s="13">
+      <c r="A9" s="15">
         <v>8.0</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="16">
         <v>1.0</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="G9" s="14"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G9" s="16"/>
     </row>
     <row r="10">
-      <c r="A10" s="13">
+      <c r="A10" s="15">
         <v>9.0</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="16">
         <v>1.0</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="G10" s="14"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="G10" s="16"/>
     </row>
     <row r="11">
       <c r="A11" s="2">
@@ -3587,17 +3913,17 @@
         <v>2.0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>191</v>
+        <v>252</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>201</v>
+        <v>262</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>202</v>
+        <v>263</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>203</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12">
@@ -3610,13 +3936,13 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>204</v>
+        <v>265</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>205</v>
+        <v>266</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>206</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13">
@@ -3629,84 +3955,84 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="18"/>
+      <c r="F13" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="20"/>
     </row>
     <row r="14">
-      <c r="A14" s="13">
+      <c r="A14" s="15">
         <v>13.0</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="16">
         <v>3.0</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>210</v>
+      <c r="C14" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="13">
+      <c r="A15" s="15">
         <v>14.0</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="16">
         <v>3.0</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>213</v>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="13">
+      <c r="A16" s="15">
         <v>15.0</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="16">
         <v>3.0</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>216</v>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="13">
+      <c r="A17" s="15">
         <v>16.0</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="16">
         <v>3.0</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="G17" s="14"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="G17" s="16"/>
     </row>
     <row r="18">
       <c r="A18" s="2">
@@ -3716,14 +4042,14 @@
         <v>4.0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>218</v>
+        <v>279</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>219</v>
+        <v>280</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>220</v>
+        <v>281</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -3737,10 +4063,10 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>221</v>
+        <v>282</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>222</v>
+        <v>283</v>
       </c>
       <c r="G19" s="3"/>
     </row>
@@ -3754,10 +4080,10 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>224</v>
+        <v>285</v>
       </c>
       <c r="G20" s="3"/>
     </row>
@@ -3771,10 +4097,10 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>225</v>
+        <v>286</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>226</v>
+        <v>287</v>
       </c>
       <c r="G21" s="3"/>
     </row>
@@ -3788,10 +4114,10 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>227</v>
+        <v>288</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>228</v>
+        <v>289</v>
       </c>
       <c r="G22" s="3"/>
     </row>
@@ -3806,77 +4132,77 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="13">
+      <c r="A24" s="15">
         <v>23.0</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="16">
         <v>5.0</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="G24" s="14"/>
+      <c r="C24" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="G24" s="16"/>
     </row>
     <row r="25">
-      <c r="A25" s="13">
+      <c r="A25" s="15">
         <v>24.0</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="16">
         <v>5.0</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="G25" s="14"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="G25" s="16"/>
     </row>
     <row r="26">
-      <c r="A26" s="13">
+      <c r="A26" s="15">
         <v>25.0</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="16">
         <v>5.0</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="G26" s="14"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="G26" s="16"/>
     </row>
     <row r="27">
-      <c r="A27" s="13">
+      <c r="A27" s="15">
         <v>26.0</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="16">
         <v>5.0</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="G27" s="14"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="G27" s="16"/>
     </row>
     <row r="28">
       <c r="A28" s="2">
@@ -3886,14 +4212,14 @@
         <v>6.0</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>236</v>
+        <v>297</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>237</v>
+        <v>298</v>
       </c>
       <c r="G28" s="3"/>
     </row>
@@ -3907,10 +4233,10 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>238</v>
+        <v>299</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>239</v>
+        <v>300</v>
       </c>
       <c r="G29" s="3"/>
     </row>
@@ -3924,10 +4250,10 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>240</v>
+        <v>301</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>241</v>
+        <v>302</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -3941,10 +4267,10 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>235</v>
+        <v>296</v>
       </c>
       <c r="G31" s="3"/>
     </row>
@@ -3959,7 +4285,7 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>242</v>
+        <v>303</v>
       </c>
       <c r="G32" s="3"/>
     </row>

</xml_diff>